<commit_message>
Ajout conception actuelle; screens pour présentation.
</commit_message>
<xml_diff>
--- a/01_Conception/Dictionnaire_de_données/Dictionnaire_de_donnees.xlsx
+++ b/01_Conception/Dictionnaire_de_données/Dictionnaire_de_donnees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomfouet/Documents/Git/Github/LIDEM/TP/TP_SYMFONY_CAMPING/TP_JS_O_API_Camping/01_Conception/Dictionnaire_de_données/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC29203-5E9E-CB49-BB85-7627CD7EB1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEF7F0F-D26C-A841-90BD-5F394E276D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" xr2:uid="{C3CF560D-D6D9-F249-948B-BEE84DC250CC}"/>
   </bookViews>
@@ -337,19 +337,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,7 +838,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,10 +874,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C3">
@@ -889,10 +888,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C4">
@@ -903,10 +902,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C5">
@@ -917,10 +916,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C6">
@@ -931,10 +930,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D7" t="s">
@@ -942,10 +941,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C8">
@@ -956,10 +955,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C9">
@@ -970,10 +969,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C10">
@@ -984,10 +983,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C11">
@@ -1001,7 +1000,7 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D13" t="s">
@@ -1012,7 +1011,7 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C14">
@@ -1026,7 +1025,7 @@
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D16" t="s">
@@ -1037,7 +1036,7 @@
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C17">
@@ -1051,7 +1050,7 @@
       <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D18" t="s">
@@ -1062,7 +1061,7 @@
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D19" t="s">
@@ -1073,7 +1072,7 @@
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D20" t="s">
@@ -1084,7 +1083,7 @@
       <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
@@ -1095,7 +1094,7 @@
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D22" t="s">
@@ -1106,7 +1105,7 @@
       <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D24" t="s">
@@ -1117,7 +1116,7 @@
       <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D25" t="s">
@@ -1128,7 +1127,7 @@
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D26" t="s">
@@ -1139,7 +1138,7 @@
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D27" t="s">
@@ -1150,7 +1149,7 @@
       <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D28" t="s">
@@ -1161,7 +1160,7 @@
       <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D29" t="s">
@@ -1172,7 +1171,7 @@
       <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D30" t="s">
@@ -1183,7 +1182,7 @@
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C31">
@@ -1197,7 +1196,7 @@
       <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D32" t="s">
@@ -1208,7 +1207,7 @@
       <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D33" t="s">
@@ -1219,7 +1218,7 @@
       <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D35" t="s">
@@ -1230,7 +1229,7 @@
       <c r="A36" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D36" t="s">
@@ -1241,7 +1240,7 @@
       <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D37" t="s">
@@ -1252,7 +1251,7 @@
       <c r="A38" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D38" t="s">
@@ -1263,7 +1262,7 @@
       <c r="A40" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D40" t="s">
@@ -1274,7 +1273,7 @@
       <c r="A41" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C41">
@@ -1288,7 +1287,7 @@
       <c r="A42" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D42" t="s">
@@ -1299,7 +1298,7 @@
       <c r="A43" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D43" t="s">
@@ -1310,7 +1309,7 @@
       <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D45" t="s">
@@ -1321,7 +1320,7 @@
       <c r="A46" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C46">
@@ -1335,7 +1334,7 @@
       <c r="A48" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D48" t="s">
@@ -1346,7 +1345,7 @@
       <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D49" t="s">
@@ -1357,7 +1356,7 @@
       <c r="A50" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1368,7 +1367,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27159740-83FD-6645-8568-E35CCE71C1E8}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C11"/>
@@ -1385,7 +1384,7 @@
     <col min="7" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1425,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1441,7 +1440,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -1454,7 +1453,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>7</v>
@@ -1467,7 +1466,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
@@ -1480,7 +1479,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>17</v>
@@ -1493,12 +1492,12 @@
       <c r="F7" s="4"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="4"/>
@@ -1506,12 +1505,12 @@
       <c r="F8" s="4"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="4"/>
@@ -1519,12 +1518,12 @@
       <c r="F9" s="4"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="4">
@@ -1534,19 +1533,19 @@
       <c r="F10" s="4"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1555,7 +1554,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1570,7 +1569,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
         <v>23</v>
@@ -1583,7 +1582,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>24</v>
@@ -1595,9 +1594,8 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
@@ -1609,9 +1607,8 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
         <v>26</v>
@@ -1623,9 +1620,8 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
         <v>27</v>
@@ -1637,9 +1633,8 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>28</v>
@@ -1650,10 +1645,8 @@
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>29</v>
@@ -1665,9 +1658,8 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>30</v>
@@ -1679,9 +1671,8 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1689,9 +1680,8 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -1705,9 +1695,8 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>32</v>
@@ -1718,36 +1707,31 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="5" t="s">
         <v>34</v>
@@ -1759,9 +1743,8 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="5" t="s">
         <v>35</v>
@@ -1773,35 +1756,31 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
         <v>13</v>
@@ -1813,9 +1792,8 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
         <v>14</v>
@@ -1827,9 +1805,8 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
         <v>38</v>
@@ -1840,10 +1817,8 @@
       <c r="D33" s="4"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="5" t="s">
         <v>37</v>
@@ -1855,9 +1830,8 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1865,25 +1839,23 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1891,25 +1863,23 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1917,9 +1887,8 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>45</v>
       </c>
@@ -1930,10 +1899,8 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1941,7 +1908,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1949,7 +1916,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1957,7 +1924,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1965,7 +1932,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>

</xml_diff>